<commit_message>
added condition randomization to orders
</commit_message>
<xml_diff>
--- a/editable/Orders/PAR01_RUN01.xlsx
+++ b/editable/Orders/PAR01_RUN01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CulhmanLab\Documents\GitHub\Zoom_ToM\editable\Orders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evade\Documents\GitHub\Zoom_ToM\editable\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB7A87E-FE54-4AAA-AFFA-03DEC437A400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AA3277-0E42-4957-B391-368071A41F1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{C5687CB1-4EE8-4A5B-BACE-F200205D7D06}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{C5687CB1-4EE8-4A5B-BACE-F200205D7D06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Question</t>
   </si>
   <si>
-    <t>RunType</t>
+    <t>ConditionType</t>
   </si>
 </sst>
 </file>
@@ -396,12 +396,12 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -420,202 +420,250 @@
         <v>38</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>37</v>
+      </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
       <c r="C7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>19</v>
+      </c>
       <c r="C8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>24</v>
+      </c>
       <c r="C9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
       <c r="C10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
       <c r="C11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
       <c r="C12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
       <c r="C14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G14">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>29</v>
+      </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16">
+        <v>35</v>
+      </c>
       <c r="C16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G16">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17">
+        <v>22</v>
+      </c>
       <c r="C17">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G17">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18">
+        <v>33</v>
+      </c>
       <c r="C18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G18">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19">
+        <v>31</v>
+      </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G19">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20">
+        <v>21</v>
+      </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <v>18</v>

</xml_diff>

<commit_message>
added unity commands to main script
</commit_message>
<xml_diff>
--- a/editable/Orders/PAR01_RUN01.xlsx
+++ b/editable/Orders/PAR01_RUN01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evade\Documents\GitHub\Zoom_ToM\editable\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7C2276-59EA-4324-86B0-DBFFB3FCEDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96734B50-CF19-4034-9ED4-17BA8793CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{FC6C8707-799B-4B80-8D55-E991A8407F1C}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{FC6C8707-799B-4B80-8D55-E991A8407F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C21"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,10 +428,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -439,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -450,10 +450,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -461,10 +461,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -472,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -483,10 +483,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -494,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -505,7 +505,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -516,10 +516,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -527,7 +527,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -538,10 +538,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -549,7 +549,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -560,10 +560,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -582,10 +582,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -593,10 +593,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -604,7 +604,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -615,10 +615,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -626,10 +626,10 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>